<commit_message>
All metrics calculated for residential
</commit_message>
<xml_diff>
--- a/Data/META_data_consumers_1300_FLUVIUS.xlsx
+++ b/Data/META_data_consumers_1300_FLUVIUS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fiasa\Documents\KUL\Thesis\Code\Thesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927BF2F2-CE78-461E-846F-439163654C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3CD989-B92F-4072-A628-906408B8D96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{5482777D-7807-4575-A963-DBC2A7007DD8}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="1325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="1327">
   <si>
     <t>ID</t>
   </si>
@@ -4070,6 +4070,12 @@
   </si>
   <si>
     <t>W2:W93</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -4166,18 +4172,6 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -4193,6 +4187,18 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -4668,7 +4674,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5576,14 +5582,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C9239B3-B494-4101-A483-671DCA2F8829}" name="Tabel2" displayName="Tabel2" ref="A1:S301" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C9239B3-B494-4101-A483-671DCA2F8829}" name="Tabel2" displayName="Tabel2" ref="A1:S301" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:S301" xr:uid="{9C9239B3-B494-4101-A483-671DCA2F8829}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S301">
     <sortCondition ref="E1:E301"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{C80A9CE4-10D9-4773-B29B-F8F292395AED}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{D83423F1-B86E-4A57-9FC5-DF0AD23DC7F8}" name="consumerID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D83423F1-B86E-4A57-9FC5-DF0AD23DC7F8}" name="consumerID" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{65192D6F-DD8E-455A-BB57-EA64B6753890}" name="ID2"/>
     <tableColumn id="4" xr3:uid="{D7C9D4DA-2372-4DDB-9692-3BB2F482FD62}" name="aggregate_net_consumption"/>
     <tableColumn id="5" xr3:uid="{FBBB5B91-F845-44BE-BCC3-E289784392A6}" name="aggregate_consumption"/>
@@ -82736,8 +82742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402235CD-2EF7-4696-8481-1499275FE4E5}">
   <dimension ref="A1:AL301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X5" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="AG22" sqref="AG22"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="90" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="D288" sqref="D288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -84214,6 +84220,9 @@
         <f t="shared" si="0"/>
         <v>3.6666666666666667E-2</v>
       </c>
+      <c r="AB21">
+        <v>0.25</v>
+      </c>
       <c r="AC21" s="6" t="s">
         <v>1319</v>
       </c>
@@ -84296,6 +84305,9 @@
         <f t="shared" si="0"/>
         <v>2.3333333333333334E-2</v>
       </c>
+      <c r="AB22">
+        <v>0.5</v>
+      </c>
       <c r="AC22" s="6" t="s">
         <v>1320</v>
       </c>
@@ -84378,6 +84390,9 @@
         <f t="shared" si="0"/>
         <v>3.6666666666666667E-2</v>
       </c>
+      <c r="AB23">
+        <v>0.75</v>
+      </c>
       <c r="AC23" s="6" t="s">
         <v>1321</v>
       </c>
@@ -84459,6 +84474,12 @@
       <c r="Z24">
         <f t="shared" si="0"/>
         <v>2.3333333333333334E-2</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>1326</v>
+      </c>
+      <c r="AC24" s="6" t="s">
+        <v>1325</v>
       </c>
       <c r="AD24">
         <f>QUARTILE(E2:E301,4)</f>

</xml_diff>